<commit_message>
added CountryCode reference, and functions to calculate shares of Emigrants and Immigrants, also worked on Vis and did some weird Map-Experiments
</commit_message>
<xml_diff>
--- a/Data/Created/mergeBLIxWM.xlsx
+++ b/Data/Created/mergeBLIxWM.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27320" windowHeight="14820" tabRatio="500"/>
+    <workbookView xWindow="20" yWindow="460" windowWidth="27320" windowHeight="14820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -988,8 +989,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:HH37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="75" zoomScaleNormal="87" zoomScalePageLayoutView="87" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="75" zoomScaleNormal="87" zoomScalePageLayoutView="87" workbookViewId="0">
+      <selection activeCell="O41" sqref="O41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -25049,6 +25050,18 @@
     <sortCondition descending="1" ref="B2:B37"/>
   </sortState>
   <conditionalFormatting sqref="B2:B37 E2:E37 H2:H37 K2:K37 N2:N37 Q2:Q37 T2:T37 W2:W37 Z2:Z37 AC2:AC37 AF2:AF37 AI2:AI37 AL2:AL37 AO2:AO37 AR2:AR37 AU2:AU37 AX2:AX37 BA2:BA37 BD2:BD37 BG2:BG37 BJ2:BJ37 BM2:BM37 BP2:BP37 BS2:BS37 BV2:BV37 BY2:BY37 CB2:CB37 CE2:CE37 CH2:CH37 CK2:CK37 CN2:CN37 CQ2:CQ37 CT2:CT37 CW2:CW37 CZ2:CZ37 DC2:DC37 DF2:DF37 DI2:DI37 DL2:DL37 DO2:DO37 DR2:DR37 DU2:DU37 DX2:DX37 EA2:EA37 ED2:ED37 EG2:EG37 EJ2:EJ37 EM2:EM37 EP2:EP37 ES2:ES37 EV2:EV37 EY2:EY37 FB2:FB37 FE2:FE37 FH2:FH37 FK2:FK37 FN2:FN37 FQ2:FQ37 FT2:FT37 FW2:FW37 FZ2:FZ37 GC2:GC37 GF2:GF37 GI2:GI37 GL2:GL37 GO2:GO37 GR2:GR37 GU2:GU37 GX2:GX37 HA2:HA37 HD2:HD37 HG2:HG37">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C37 F2:F37 I2:I37 L2:L37 O2:O37 R2:R37 U2:U37 X2:X37 AA2:AA37 AD2:AD37 AG2:AG37 AJ2:AJ37 AM2:AM37 AP2:AP37 AS2:AS37 AV2:AV37 AY2:AY37 BB2:BB37 BE2:BE37 BH2:BH37 BK2:BK37 BN2:BN37 BQ2:BQ37 BT2:BT37 BW2:BW37 BZ2:BZ37 CC2:CC37 CF2:CF37 CI2:CI37 CL2:CL37 CO2:CO37 CR2:CR37 CU2:CU37 CX2:CX37 DA2:DA37 DD2:DD37 DG2:DG37 DJ2:DJ37 DM2:DM37 DP2:DP37 DS2:DS37 DV2:DV37 DY2:DY37 EB2:EB37 EE2:EE37 EH2:EH37 EK2:EK37 EN2:EN37 EQ2:EQ37 ET2:ET37 EW2:EW37 EZ2:EZ37 FC2:FC37 FF2:FF37 FI2:FI37 FL2:FL37 FO2:FO37 FR2:FR37 FU2:FU37 FX2:FX37 GA2:GA37 GD2:GD37 GG2:GG37 GJ2:GJ37 GM2:GM37 GP2:GP37 GS2:GS37 GV2:GV37 GY2:GY37 HB2:HB37 HE2:HE37 HH2:HH37">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -25060,7 +25073,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C37 F2:F37 I2:I37 L2:L37 O2:O37 R2:R37 U2:U37 X2:X37 AA2:AA37 AD2:AD37 AG2:AG37 AJ2:AJ37 AM2:AM37 AP2:AP37 AS2:AS37 AV2:AV37 AY2:AY37 BB2:BB37 BE2:BE37 BH2:BH37 BK2:BK37 BN2:BN37 BQ2:BQ37 BT2:BT37 BW2:BW37 BZ2:BZ37 CC2:CC37 CF2:CF37 CI2:CI37 CL2:CL37 CO2:CO37 CR2:CR37 CU2:CU37 CX2:CX37 DA2:DA37 DD2:DD37 DG2:DG37 DJ2:DJ37 DM2:DM37 DP2:DP37 DS2:DS37 DV2:DV37 DY2:DY37 EB2:EB37 EE2:EE37 EH2:EH37 EK2:EK37 EN2:EN37 EQ2:EQ37 ET2:ET37 EW2:EW37 EZ2:EZ37 FC2:FC37 FF2:FF37 FI2:FI37 FL2:FL37 FO2:FO37 FR2:FR37 FU2:FU37 FX2:FX37 GA2:GA37 GD2:GD37 GG2:GG37 GJ2:GJ37 GM2:GM37 GP2:GP37 GS2:GS37 GV2:GV37 GY2:GY37 HB2:HB37 HE2:HE37 HH2:HH37">
+  <conditionalFormatting sqref="D2:D37 G2:G37 J2:J37 M2:M37 P2:P37 S2:S37 V2:V37 Y2:Y37 AB2:AB37 AE2:AE37 AH2:AH37 AK2:AK37 AN2:AN37 AQ2:AQ37 AT2:AT37 AW2:AW37 AZ2:AZ37 BC2:BC37 BF2:BF37 BI2:BI37 BL2:BL37 BO2:BO37 BR2:BR37 BU2:BU37 BX2:BX37 CA2:CA37 CD2:CD37 CG2:CG37 CJ2:CJ37 CM2:CM37 CP2:CP37 CS2:CS37 CV2:CV37 CY2:CY37 DB2:DB37 DE2:DE37 DH2:DH37 DK2:DK37 DN2:DN37 DQ2:DQ37 DT2:DT37 DW2:DW37 DZ2:DZ37 EC2:EC37 EF2:EF37 EI2:EI37 EL2:EL37 EO2:EO37 ER2:ER37 EU2:EU37 EX2:EX37 FA2:FA37 FD2:FD37 FG2:FG37 FJ2:FJ37 FM2:FM37 FP2:FP37 FS2:FS37 FV2:FV37 FY2:FY37 GB2:GB37 GE2:GE37 GH2:GH37 GK2:GK37 GN2:GN37 GQ2:GQ37 GT2:GT37 GW2:GW37 GZ2:GZ37 HC2:HC37 HF2:HF37">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -25072,18 +25085,30 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D37 G2:G37 J2:J37 M2:M37 P2:P37 S2:S37 V2:V37 Y2:Y37 AB2:AB37 AE2:AE37 AH2:AH37 AK2:AK37 AN2:AN37 AQ2:AQ37 AT2:AT37 AW2:AW37 AZ2:AZ37 BC2:BC37 BF2:BF37 BI2:BI37 BL2:BL37 BO2:BO37 BR2:BR37 BU2:BU37 BX2:BX37 CA2:CA37 CD2:CD37 CG2:CG37 CJ2:CJ37 CM2:CM37 CP2:CP37 CS2:CS37 CV2:CV37 CY2:CY37 DB2:DB37 DE2:DE37 DH2:DH37 DK2:DK37 DN2:DN37 DQ2:DQ37 DT2:DT37 DW2:DW37 DZ2:DZ37 EC2:EC37 EF2:EF37 EI2:EI37 EL2:EL37 EO2:EO37 ER2:ER37 EU2:EU37 EX2:EX37 FA2:FA37 FD2:FD37 FG2:FG37 FJ2:FJ37 FM2:FM37 FP2:FP37 FS2:FS37 FV2:FV37 FY2:FY37 GB2:GB37 GE2:GE37 GH2:GH37 GK2:GK37 GN2:GN37 GQ2:GQ37 GT2:GT37 GW2:GW37 GZ2:GZ37 HC2:HC37 HF2:HF37">
+  <conditionalFormatting sqref="B2:HH37">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
+        <color theme="5"/>
+        <color theme="0"/>
+        <color rgb="FF7030A0"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>